<commit_message>
update 26-02-2020, fix 13-14 february -+ 108
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">25-02-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-02-2020</t>
   </si>
 </sst>
 </file>
@@ -233,17 +236,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,6 +654,17 @@
       </c>
       <c r="C37" s="0" t="n">
         <v>2666</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>78191</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>2718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>